<commit_message>
fix output count spreadsheet
</commit_message>
<xml_diff>
--- a/Output/Electronic Copy Counts for - Tisch Reserves - 10-30-2020.xlsx
+++ b/Output/Electronic Copy Counts for - Tisch Reserves - 10-30-2020.xlsx
@@ -368,7 +368,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S4"/>
+  <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -393,9 +393,6 @@
     <col width="20" customWidth="1" min="14" max="14"/>
     <col width="20" customWidth="1" min="15" max="15"/>
     <col width="20" customWidth="1" min="16" max="16"/>
-    <col width="20" customWidth="1" min="17" max="17"/>
-    <col width="20" customWidth="1" min="18" max="18"/>
-    <col width="20" customWidth="1" min="19" max="19"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -406,92 +403,77 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Course Code</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Course Name</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>Non-Repository - on Course</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Non-Repository Citation Matches</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Books on Course</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Electronic - Match on Course</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Physical Books on Course</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>No Electronic Version for Physical Book</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Electronic - Already on Course</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Electronic - Already on Course - Different Year</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Electronic - Already on Course - COVID Temporary Electronic Collection</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Electronic - Already on Course - COVID Temporary Electronic Collection - Different Year</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Electronic - In Collection - Add to Course</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Electronic - In Collection - Potentially Add to Course - Different Year</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Electronic - Temporarily in Collection</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Electronic - Temporarily in Collection - Different Year</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>Course Code</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>Course Name</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>Electronic - Match on Course</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>Non-Match Ebooks on Course</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>Non-Match Temporary Collection Books on Course</t>
         </is>
       </c>
     </row>
@@ -501,60 +483,53 @@
           <t>Tisch Reserves</t>
         </is>
       </c>
-      <c r="B2" t="n">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>2208-80313</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Fa20-EM-0054-01-Engineering Leadership</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
         <v>25</v>
       </c>
-      <c r="C2" t="n">
+      <c r="E2" t="n">
         <v>0</v>
       </c>
-      <c r="D2" t="n">
+      <c r="F2" t="n">
         <v>31</v>
       </c>
-      <c r="E2" t="n">
+      <c r="G2" t="n">
+        <v>3</v>
+      </c>
+      <c r="H2" t="n">
         <v>1</v>
       </c>
-      <c r="F2" t="n">
+      <c r="I2" t="n">
         <v>1</v>
-      </c>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I2" t="n">
-        <v>0</v>
       </c>
       <c r="J2" t="n">
         <v>0</v>
       </c>
       <c r="K2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M2" t="n">
         <v>2</v>
       </c>
-      <c r="L2" t="n">
+      <c r="N2" t="n">
         <v>2</v>
       </c>
-      <c r="M2" t="n">
+      <c r="O2" t="n">
         <v>0</v>
       </c>
-      <c r="N2" t="n">
-        <v>0</v>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>2208-80313</t>
-        </is>
-      </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>Fa20-EM-0054-01-Engineering Leadership</t>
-        </is>
-      </c>
-      <c r="Q2" t="n">
-        <v>3</v>
-      </c>
-      <c r="R2" t="n">
-        <v>0</v>
-      </c>
-      <c r="S2" t="n">
+      <c r="P2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -595,11 +570,27 @@
         <v/>
       </c>
       <c r="K4" s="2">
+        <f> SUM(K1:K2)</f>
+        <v/>
+      </c>
+      <c r="L4" s="2">
+        <f> SUM(L1:L2)</f>
+        <v/>
+      </c>
+      <c r="M4">
         <f> SUM(M1:M2)</f>
         <v/>
       </c>
-      <c r="L4" s="2">
+      <c r="N4">
         <f> SUM(N1:N2)</f>
+        <v/>
+      </c>
+      <c r="O4">
+        <f> SUM(O1:P2)</f>
+        <v/>
+      </c>
+      <c r="P4">
+        <f> SUM(P1:P2)</f>
         <v/>
       </c>
     </row>

</xml_diff>